<commit_message>
Rapport.md /  Planification.md / JDT
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07463CB-A8D3-4A1C-8C27-03B88AC60837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C01CD-1125-491A-9D8D-5A14308F7200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Auteur:</t>
   </si>
@@ -160,6 +160,14 @@
   </si>
   <si>
     <t>Création des user stories et Acceptance criteria</t>
+  </si>
+  <si>
+    <t>Rapport.md /  Planification.md / JDT</t>
+  </si>
+  <si>
+    <t>Rapport /  Planification; Création des fichiers et organisation des dossiers pour le projet. apport : Rédaction complète du rapport du projet, incluant objectifs, domaine, analyse, réalisation, tests et conclusion.
+Planification : Élaboration du plan sur 8 semaines avec tâches, livrables et marges pour les imprévus.
+JDT : Tenue du journal de travail pour suivre l’avancement, les difficultés rencontrées et les solutions apportées.</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1180,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2096,7 +2104,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.54545454545454541</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2105,7 +2113,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45454545454545453</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4294,7 +4302,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4349,7 +4357,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 50 minutes</v>
+        <v>2 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4368,11 +4376,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4519,17 +4527,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="str">
+    <row r="11" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="34"/>
+        <v>35</v>
+      </c>
+      <c r="B11" s="34">
+        <v>45898</v>
+      </c>
       <c r="C11" s="35"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="40"/>
+      <c r="D11" s="36">
+        <v>40</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>39</v>
+      </c>
       <c r="M11" t="s">
         <v>4</v>
       </c>
@@ -10990,7 +11008,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.54545454545454541</v>
+        <v>0.4</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11085,11 +11103,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11097,11 +11115,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 50 min</v>
+        <v>1 h 30 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.45454545454545453</v>
+        <v>0.6</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11157,22 +11175,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 50 min</v>
+        <v>2 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>2.0833333333333332E-2</v>
+        <v>2.8409090909090908E-2</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11216,6 +11234,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11224,15 +11251,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11437,6 +11455,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11445,14 +11471,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Codage creation du projet vs, premier graphique
Début du codage du projet : création et modélisation des Windows Forms, création des classes, et première mise en place d’une interface graphique évolutive.
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B210B-374C-4017-8F5F-1D9B4585B7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5565BF1A-4699-4FD6-B468-B9B01EEDDD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Auteur:</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.youtube.com/watch?v=HGF1fm1vmIk&amp;ab_channel=IndustrialITandAutomation   Tooltip: https://www.w3schools.com/css/css_tooltip.asp   windowsforms: https://stackoverflow.com/questions/29024910/how-to-design-a-custom-close-minimize-and-maximize-button-in-windows-form-appli </t>
+  </si>
+  <si>
+    <t>Début du codage du projet : création et modélisation des Windows Forms, création des classes, et première mise en place d’une interface graphique évolutive.</t>
+  </si>
+  <si>
+    <t>System.Text.Json / ScottPlot</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1216,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2140,16 +2146,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.34482758620689657</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13793103448275862</c:v>
+                  <c:v>0.21875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51724137931034486</c:v>
+                  <c:v>0.46875</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4337,8 +4343,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4399,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>4 heures 50 minutes</v>
+        <v>5 heures 20 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4412,11 +4418,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>290</v>
+        <v>320</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4681,17 +4687,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="str">
+    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="63">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="34"/>
+        <v>36</v>
+      </c>
+      <c r="B15" s="34">
+        <v>45905</v>
+      </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="40"/>
+      <c r="D15" s="36">
+        <v>30</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="N15">
         <v>8</v>
       </c>
@@ -11078,7 +11094,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.34482758620689657</v>
+        <v>0.3125</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11099,11 +11115,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11111,11 +11127,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 40 min</v>
+        <v>1 h 10 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.13793103448275862</v>
+        <v>0.21875</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11189,7 +11205,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.51724137931034486</v>
+        <v>0.46875</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11245,22 +11261,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>290</v>
+        <v>320</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 50 min</v>
+        <v>5 h 20 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.2013888888888889</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
src/data (data samples); src/(project)first chart was made
src/data(btc_Xdays.json, eth_Xdays.json, pepe_Xdays.json, solana_Xdays.json)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5565BF1A-4699-4FD6-B468-B9B01EEDDD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D991F1CB-9B97-4974-9B2E-34CC4C57BF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Auteur:</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Réfléxion sur le but et moyens à l'aide desquels attenir les goals est pas seulement réel, mais qui correspond à ma manniere et la thème de Crypto monnaies, Amélioration de Readme.md, ajout des notion nésaiser(utilité de mon projet, son but, réelistion, test, tech stack); choix du thème et API</t>
   </si>
   <si>
-    <t>https://www.coingecko.com/en/api?utm_source=chatgpt.com</t>
-  </si>
-  <si>
     <t>Création de mon mon repos GitHub privé, Une structure de fichiers organisée a été mise en place afin d’assurer une bonne lisibilité et une gestion efficace du code et des    ressources(          documentation/ — pour tous les documents liés au projet
 readme.md — fichier de présentation du projet-Rapport | .gitignore
 Début de la planification des tâches dans le JDT</t>
@@ -192,6 +189,15 @@
   </si>
   <si>
     <t>System.Text.Json / ScottPlot</t>
+  </si>
+  <si>
+    <t>https://www.coingecko.com/en/api?</t>
+  </si>
+  <si>
+    <t>Premier graphique; faire connaissance sur des fonctionnalités principales-nécessaires; +json extrait des cryptos monnaies</t>
+  </si>
+  <si>
+    <t>{"error":{"status":{"timestamp":"2025-09-12T12:30:06.778+00:00","error_code":10012,"error_message":"Your request exceeds the allowed time range. Public API users are limited to querying historical data within the past 365 days. Upgrade to a paid plan to enjoy full historical data access: https://www.coingecko.com/en/api/pricing. "}}}</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1222,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2146,16 +2152,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3125</c:v>
+                  <c:v>0.26315789473684209</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21875</c:v>
+                  <c:v>0.34210526315789475</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46875</c:v>
+                  <c:v>0.39473684210526316</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4343,8 +4349,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4399,7 +4405,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 20 minutes</v>
+        <v>6 heures 20 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4414,7 +4420,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -4422,7 +4428,7 @@
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4492,10 +4498,10 @@
         <v>4</v>
       </c>
       <c r="F8" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="39" t="s">
         <v>36</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>37</v>
       </c>
       <c r="M8" t="s">
         <v>2</v>
@@ -4523,7 +4529,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="40" t="s">
         <v>33</v>
@@ -4556,8 +4562,8 @@
       <c r="F10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="39" t="s">
-        <v>35</v>
+      <c r="G10" s="85" t="s">
+        <v>48</v>
       </c>
       <c r="M10" t="s">
         <v>3</v>
@@ -4585,10 +4591,10 @@
         <v>4</v>
       </c>
       <c r="F11" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="40" t="s">
         <v>39</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>40</v>
       </c>
       <c r="M11" t="s">
         <v>4</v>
@@ -4616,10 +4622,10 @@
         <v>4</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M12" t="s">
         <v>28</v>
@@ -4647,10 +4653,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N13">
         <v>6</v>
@@ -4675,10 +4681,10 @@
         <v>19</v>
       </c>
       <c r="F14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="39" t="s">
         <v>44</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>45</v>
       </c>
       <c r="N14">
         <v>7</v>
@@ -4703,10 +4709,10 @@
         <v>19</v>
       </c>
       <c r="F15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="40" t="s">
         <v>47</v>
-      </c>
-      <c r="G15" s="40" t="s">
-        <v>48</v>
       </c>
       <c r="N15">
         <v>8</v>
@@ -4715,27 +4721,39 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="str">
+    <row r="16" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="62">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
+        <v>37</v>
+      </c>
+      <c r="B16" s="30">
+        <v>45912</v>
+      </c>
+      <c r="C16" s="31">
+        <v>1</v>
+      </c>
       <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="39"/>
+      <c r="E16" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>50</v>
+      </c>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
+        <v>37</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45912</v>
+      </c>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
       <c r="E17" s="37"/>
@@ -4746,11 +4764,13 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
+        <v>37</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45912</v>
+      </c>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
       <c r="E18" s="33"/>
@@ -4761,11 +4781,13 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>37</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45912</v>
+      </c>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
       <c r="E19" s="37"/>
@@ -10982,11 +11004,12 @@
   <hyperlinks>
     <hyperlink ref="G13" r:id="rId1" display="https://www.youtube.com/watch?v=HGF1fm1vmIk&amp;ab_channel=IndustrialITandAutomation" xr:uid="{336CBD97-FBE6-4DA0-92F1-7E19F61FE3AA}"/>
     <hyperlink ref="G12" r:id="rId2" xr:uid="{160CB3A4-60AC-4C67-9742-E843A97D81B7}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{0F91120E-3455-4E0F-8C60-6729CE2C909C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11094,7 +11117,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.3125</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11111,7 +11134,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -11119,7 +11142,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11127,11 +11150,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>1 h 10 min</v>
+        <v>2 h 10 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.21875</v>
+        <v>0.34210526315789475</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11205,7 +11228,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.46875</v>
+        <v>0.39473684210526316</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11257,7 +11280,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
@@ -11265,18 +11288,18 @@
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 20 min</v>
+        <v>6 h 20 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.22222222222222221</v>
+        <v>0.2638888888888889</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
src/PTL_Crypto(PlotManager) gérer le graphique-apparence;  src/PTL_Crypto(ApiClient) reçoit des réponses(json)  par lien ,src/PTL_Crypto(Form1) Load crypto from main form using  textbox and buttons, JDT mis à jour
comments💚
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D991F1CB-9B97-4974-9B2E-34CC4C57BF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A609BA89-82ED-4B6A-9BBE-A397DE370473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Auteur:</t>
   </si>
@@ -198,6 +198,21 @@
   </si>
   <si>
     <t>{"error":{"status":{"timestamp":"2025-09-12T12:30:06.778+00:00","error_code":10012,"error_message":"Your request exceeds the allowed time range. Public API users are limited to querying historical data within the past 365 days. Upgrade to a paid plan to enjoy full historical data access: https://www.coingecko.com/en/api/pricing. "}}}</t>
+  </si>
+  <si>
+    <t>Button import importation de json,  parsing json, pour créer un graphique,</t>
+  </si>
+  <si>
+    <t>features button import</t>
+  </si>
+  <si>
+    <t>JDT mis à jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> src/PTL_Crypto(PlotManager) gérer le graphique-apparence;  src/PTL_Crypto(ApiClient) reçoit des réponses(json)  par lien ,src/PTL_Crypto(Form1) Load crypto from main form using  textbox and buttons, </t>
+  </si>
+  <si>
+    <t>ApiClient,Form1,PlotManager</t>
   </si>
 </sst>
 </file>
@@ -1222,13 +1237,13 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2152,16 +2167,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.26315789473684209</c:v>
+                  <c:v>0.20618556701030927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34210526315789475</c:v>
+                  <c:v>0.46391752577319589</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39473684210526316</c:v>
+                  <c:v>0.32989690721649484</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4349,8 +4364,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4405,7 +4420,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 20 minutes</v>
+        <v>8 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4420,15 +4435,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>380</v>
+        <v>485</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4746,7 +4761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
         <v>37</v>
@@ -4754,11 +4769,21 @@
       <c r="B17" s="34">
         <v>45912</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="40"/>
+      <c r="C17" s="35">
+        <v>1</v>
+      </c>
+      <c r="D17" s="36">
+        <v>20</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>55</v>
+      </c>
       <c r="O17">
         <v>45</v>
       </c>
@@ -4772,10 +4797,18 @@
         <v>45912</v>
       </c>
       <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="39"/>
+      <c r="D18" s="32">
+        <v>15</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="O18">
         <v>50</v>
       </c>
@@ -4789,9 +4822,15 @@
         <v>45912</v>
       </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>10</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
@@ -11117,7 +11156,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.26315789473684209</v>
+        <v>0.20618556701030927</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11134,15 +11173,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>225</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11150,11 +11189,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 10 min</v>
+        <v>3 h 45 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.34210526315789475</v>
+        <v>0.46391752577319589</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11212,11 +11251,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11224,11 +11263,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 30 min</v>
+        <v>2 h 40 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.39473684210526316</v>
+        <v>0.32989690721649484</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11280,26 +11319,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>380</v>
+        <v>485</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 20 min</v>
+        <v>8 h 05 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.2638888888888889</v>
+        <v>0.33680555555555558</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11343,15 +11382,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11360,6 +11390,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11564,14 +11603,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11580,6 +11611,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
code(FileClient class, Form1(LoadCrypto(local and api) )) [WIP]
Quand je démarre l’application, alors un graphique ScottPlot est visible. Le graphique affiche les prix du Bitcoin sur 7 jours (et autres crypto monaies) by default.
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A609BA89-82ED-4B6A-9BBE-A397DE370473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C918E42B-C25F-4CC5-874B-16F8314A71BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Auteur:</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>ApiClient,Form1,PlotManager</t>
+  </si>
+  <si>
+    <t>https://scottplot.net/cookbook/4.1/category/plottable-scatter-plot/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code(FileClient class, Form1 )     -     Quand je démarre l’application, alors un graphique ScottPlot est visible. Le graphique affiche les prix du Bitcoin sur 7 jours (et autres crypto monaies) by default. </t>
+  </si>
+  <si>
+    <t>JUST info CSV import:   https://hackernoon.com/importing-exporting-csv-and-excel-xlsx-in-net-c-applications</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1246,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>225</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2167,16 +2176,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.20618556701030927</c:v>
+                  <c:v>0.18018018018018017</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46391752577319589</c:v>
+                  <c:v>0.53153153153153154</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32989690721649484</c:v>
+                  <c:v>0.28828828828828829</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4364,8 +4373,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4420,7 +4429,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>8 heures 5 minutes</v>
+        <v>9 heures 15 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4435,15 +4444,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>485</v>
+        <v>555</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4831,53 +4840,73 @@
       <c r="F19" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="40"/>
+      <c r="G19" s="84"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="39"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45926</v>
+      </c>
+      <c r="C20" s="31">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>10</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="85" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45926</v>
+      </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
       <c r="E21" s="37"/>
       <c r="F21" s="23"/>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+    <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45926</v>
+      </c>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="39"/>
+      <c r="G22" s="39" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="str">
+      <c r="A23" s="63">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="34"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="34">
+        <v>45926</v>
+      </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
       <c r="E23" s="37"/>
@@ -11044,11 +11073,12 @@
     <hyperlink ref="G13" r:id="rId1" display="https://www.youtube.com/watch?v=HGF1fm1vmIk&amp;ab_channel=IndustrialITandAutomation" xr:uid="{336CBD97-FBE6-4DA0-92F1-7E19F61FE3AA}"/>
     <hyperlink ref="G12" r:id="rId2" xr:uid="{160CB3A4-60AC-4C67-9742-E843A97D81B7}"/>
     <hyperlink ref="G10" r:id="rId3" xr:uid="{0F91120E-3455-4E0F-8C60-6729CE2C909C}"/>
+    <hyperlink ref="G20" r:id="rId4" xr:uid="{4AC877DD-0538-4960-9300-3F6AF2D7E0D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11156,7 +11186,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.20618556701030927</v>
+        <v>0.18018018018018017</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11173,15 +11203,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>295</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11189,11 +11219,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>3 h 45 min</v>
+        <v>4 h 55 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.46391752577319589</v>
+        <v>0.53153153153153154</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11267,7 +11297,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.32989690721649484</v>
+        <v>0.28828828828828829</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11319,26 +11349,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>485</v>
+        <v>555</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>8 h 05 min</v>
+        <v>9 h 15 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.33680555555555558</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
code(PlotManager(for local and Api data))
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C918E42B-C25F-4CC5-874B-16F8314A71BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E100FE-1980-45BE-BD45-4A2749A3DB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>Auteur:</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>JUST info CSV import:   https://hackernoon.com/importing-exporting-csv-and-excel-xlsx-in-net-c-applications</t>
+  </si>
+  <si>
+    <t>code(PlotManager(for local and Api data))</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1249,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>295</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2176,16 +2179,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.18018018018018017</c:v>
+                  <c:v>0.17391304347826086</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53153153153153154</c:v>
+                  <c:v>0.54782608695652169</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28828828828828829</c:v>
+                  <c:v>0.27826086956521739</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4374,7 +4377,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4429,7 +4432,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 15 minutes</v>
+        <v>9 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4448,11 +4451,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4878,9 +4881,15 @@
         <v>45926</v>
       </c>
       <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
+      <c r="D21" s="36">
+        <v>20</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -11186,7 +11195,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.18018018018018017</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11207,11 +11216,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11219,11 +11228,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 55 min</v>
+        <v>5 h 15 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.53153153153153154</v>
+        <v>0.54782608695652169</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11297,7 +11306,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.28828828828828829</v>
+        <v>0.27826086956521739</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11353,22 +11362,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>555</v>
+        <v>575</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 15 min</v>
+        <v>9 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.38541666666666669</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11412,6 +11421,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11420,15 +11438,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11633,6 +11642,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11641,14 +11658,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Chore(JDT); code(PlotManager(Deleting,Restoring charts, Importing a JSON file))
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E100FE-1980-45BE-BD45-4A2749A3DB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E7ACE7-D441-4204-AC96-4459B82F543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Auteur:</t>
   </si>
@@ -221,10 +221,13 @@
     <t xml:space="preserve">code(FileClient class, Form1 )     -     Quand je démarre l’application, alors un graphique ScottPlot est visible. Le graphique affiche les prix du Bitcoin sur 7 jours (et autres crypto monaies) by default. </t>
   </si>
   <si>
-    <t>JUST info CSV import:   https://hackernoon.com/importing-exporting-csv-and-excel-xlsx-in-net-c-applications</t>
+    <t>code(PlotManager(for local and Api data))</t>
   </si>
   <si>
-    <t>code(PlotManager(for local and Api data))</t>
+    <t xml:space="preserve"> correction des erreurs version 4.0 -&gt; 5.0</t>
+  </si>
+  <si>
+    <t>representation des graphique coherent,Chore(JDT); code(PlotManager(Deleting,Restoring charts, Importing a JSON file))</t>
   </si>
 </sst>
 </file>
@@ -1249,13 +1252,13 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>315</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2179,16 +2182,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.17391304347826086</c:v>
+                  <c:v>0.15625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54782608695652169</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27826086956521739</c:v>
+                  <c:v>0.265625</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4375,9 +4378,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4432,7 +4435,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 35 minutes</v>
+        <v>10 heures 40 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4451,11 +4454,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>335</v>
+        <v>400</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>575</v>
+        <v>640</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4882,15 +4885,17 @@
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="62">
@@ -4901,12 +4906,16 @@
         <v>45926</v>
       </c>
       <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="39" t="s">
-        <v>58</v>
-      </c>
+      <c r="D22" s="32">
+        <v>35</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="63">
@@ -4917,9 +4926,15 @@
         <v>45926</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+      <c r="D23" s="36">
+        <v>10</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -11195,7 +11210,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.17391304347826086</v>
+        <v>0.15625</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11216,11 +11231,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>370</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11228,11 +11243,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>5 h 15 min</v>
+        <v>6 h 10 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.54782608695652169</v>
+        <v>0.578125</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11290,11 +11305,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11302,11 +11317,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 40 min</v>
+        <v>2 h 50 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.27826086956521739</v>
+        <v>0.265625</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11362,22 +11377,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>335</v>
+        <v>400</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>575</v>
+        <v>640</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 35 min</v>
+        <v>10 h 40 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.39930555555555558</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11421,15 +11436,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11438,6 +11444,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11642,14 +11657,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11658,6 +11665,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
src(Prototype API + combobox ), chore(JDT)
recherche des crypto avec combobox(GetCoinsListAsync,CoinInfo),les messages clair qui informe d'un  problème ou réussit
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E7ACE7-D441-4204-AC96-4459B82F543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF36C0B-83DA-4961-9A86-1AD578E62255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Auteur:</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>representation des graphique coherent,Chore(JDT); code(PlotManager(Deleting,Restoring charts, Importing a JSON file))</t>
+  </si>
+  <si>
+    <t>recherche des crypto avec combobox,les messages clair qui informe d'un  problème ou réussit</t>
+  </si>
+  <si>
+    <t>src(Prototype API + combobox ), chore(JDT)</t>
   </si>
 </sst>
 </file>
@@ -1252,13 +1258,13 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>370</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>170</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2182,16 +2188,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.15625</c:v>
+                  <c:v>0.14492753623188406</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.578125</c:v>
+                  <c:v>0.59420289855072461</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.265625</c:v>
+                  <c:v>0.2608695652173913</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4379,8 +4385,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4435,7 +4441,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>10 heures 40 minutes</v>
+        <v>11 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4454,11 +4460,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>640</v>
+        <v>690</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4938,23 +4944,35 @@
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="str">
+      <c r="A24" s="62">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="B24" s="30">
+        <v>45933</v>
+      </c>
       <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="39"/>
+      <c r="D24" s="32">
+        <v>40</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="str">
+      <c r="A25" s="63">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="34">
+        <v>45933</v>
+      </c>
       <c r="C25" s="35"/>
       <c r="D25" s="36"/>
       <c r="E25" s="37"/>
@@ -4962,11 +4980,13 @@
       <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="62" t="str">
+      <c r="A26" s="62">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="B26" s="30">
+        <v>45933</v>
+      </c>
       <c r="C26" s="31"/>
       <c r="D26" s="32"/>
       <c r="E26" s="33"/>
@@ -4974,15 +4994,23 @@
       <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="str">
+      <c r="A27" s="63">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="B27" s="34">
+        <v>45933</v>
+      </c>
       <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="23"/>
+      <c r="D27" s="36">
+        <v>10</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -11210,7 +11238,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.15625</v>
+        <v>0.14492753623188406</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11231,11 +11259,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>370</v>
+        <v>410</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11243,11 +11271,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>6 h 10 min</v>
+        <v>6 h 50 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.578125</v>
+        <v>0.59420289855072461</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11305,11 +11333,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11317,11 +11345,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 50 min</v>
+        <v>3 h 00 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.265625</v>
+        <v>0.2608695652173913</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11377,22 +11405,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>640</v>
+        <v>690</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>10 h 40 min</v>
+        <v>11 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.44444444444444442</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
dans graphique les dates claires et correctes + try catch + Comments pour classes
try catch pour éviter des erreurs leur fonctionnement d'api
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF36C0B-83DA-4961-9A86-1AD578E62255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E53081D-5587-4065-A466-DA4C26C665FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Auteur:</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>src(Prototype API + combobox ), chore(JDT)</t>
+  </si>
+  <si>
+    <t>https://scottplot.net/cookbook/5.0/Scatter/    formsPlot1.Plot.Axes.DateTimeTicksBottom();</t>
+  </si>
+  <si>
+    <t>dans graphique les dates claires et correctes + try catch  pour éviter des erreurs leur fonctionnement d'api + Comments pour classes</t>
+  </si>
+  <si>
+    <t>revue des commentaires de prof correction et addaptation des erreurs</t>
+  </si>
+  <si>
+    <t>feedback</t>
   </si>
 </sst>
 </file>
@@ -1255,10 +1267,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>410</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2188,16 +2200,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.14492753623188406</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59420289855072461</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2608695652173913</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4386,7 +4398,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4441,7 +4453,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>11 heures 30 minutes</v>
+        <v>12 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4460,11 +4472,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>450</v>
+        <v>510</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>690</v>
+        <v>750</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4953,16 +4965,16 @@
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="32">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G24" s="39" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -4974,12 +4986,20 @@
         <v>45933</v>
       </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="40"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="36">
+        <v>50</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="84" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="62">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
         <v>40</v>
@@ -4988,10 +5008,18 @@
         <v>45933</v>
       </c>
       <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="39"/>
+      <c r="D26" s="32">
+        <v>30</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="63">
@@ -11222,11 +11250,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11234,11 +11262,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>1 h 40 min</v>
+        <v>2 h 00 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.14492753623188406</v>
+        <v>0.16</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11259,11 +11287,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>450</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11271,11 +11299,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>6 h 50 min</v>
+        <v>7 h 30 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.59420289855072461</v>
+        <v>0.6</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11349,7 +11377,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.2608695652173913</v>
+        <v>0.24</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11405,22 +11433,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>450</v>
+        <v>510</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>690</v>
+        <v>750</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>11 h 30 min</v>
+        <v>12 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.47916666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
unit test (CryptoPrice object)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E53081D-5587-4065-A466-DA4C26C665FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADE8644-B7ED-42B2-AA53-CF923B8A98DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>Auteur:</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>feedback</t>
+  </si>
+  <si>
+    <t>unit test (CryptoPrice object)</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1276,7 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>180</c:v>
@@ -2200,16 +2203,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.16</c:v>
+                  <c:v>0.15384615384615385</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.57692307692307687</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.8461538461538464E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23076923076923078</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4398,7 +4401,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29:F30"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4453,7 +4456,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>12 heures 30 minutes</v>
+        <v>13 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4472,11 +4475,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>750</v>
+        <v>780</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5031,26 +5034,34 @@
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="36">
+        <v>30</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="40"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="62">
+        <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
+        <v>40</v>
+      </c>
+      <c r="B28" s="30">
+        <v>45933</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="32">
         <v>10</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E28" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F28" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="40"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="str">
-        <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="22"/>
       <c r="G28" s="39"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -11266,7 +11277,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.16</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11303,7 +11314,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.6</v>
+        <v>0.57692307692307687</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11324,11 +11335,11 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E8" s="76" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11336,11 +11347,11 @@
       </c>
       <c r="F8" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>0 h 30 min</v>
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11377,7 +11388,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.24</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11433,22 +11444,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>750</v>
+        <v>780</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>12 h 30 min</v>
+        <v>13 h 00 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.52083333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11492,6 +11503,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11500,15 +11520,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11713,6 +11724,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11721,14 +11740,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
comments in all code, amelioreation d'expliquation du code (summary...)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7766D80-C64B-4B66-8CC4-96A06AE06A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A6223-1FE1-42C2-A0EA-457D23CBC8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>Auteur:</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>Ajouter la persistance de l’état de l’application (local JSON)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'analyse du feedback avec professeur </t>
+  </si>
+  <si>
+    <t>comments in all code, amelioreation d'expliquation du code (summary...)</t>
+  </si>
+  <si>
+    <t>retouches du readme, Fix links and improve README formatting</t>
   </si>
 </sst>
 </file>
@@ -1317,16 +1326,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>800</c:v>
+                  <c:v>845</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>275</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1393,6 +1402,7 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1400,7 +1410,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1766,6 +1775,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1773,7 +1783,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2250,16 +2259,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.125475285171103E-2</c:v>
+                  <c:v>0.10071942446043165</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60836501901140683</c:v>
+                  <c:v>0.6079136690647482</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.125475285171103E-2</c:v>
+                  <c:v>8.6330935251798566E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20912547528517111</c:v>
+                  <c:v>0.20503597122302158</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2417,6 +2426,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2424,7 +2434,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4447,8 +4456,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4503,7 +4512,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>21 heures 55 minutes</v>
+        <v>23 heures 10 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4522,11 +4531,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>775</v>
+        <v>850</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>1315</v>
+        <v>1390</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5342,47 +5351,73 @@
       <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="str">
+      <c r="A40" s="62">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B40" s="30">
+        <v>45961</v>
+      </c>
       <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="22"/>
+      <c r="D40" s="32">
+        <v>20</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G40" s="39"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="63" t="str">
+      <c r="A41" s="63">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B41" s="34">
+        <v>45961</v>
+      </c>
       <c r="C41" s="35"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="22"/>
+      <c r="D41" s="36">
+        <v>45</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="G41" s="40"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="62" t="str">
+      <c r="A42" s="62">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B42" s="30">
+        <v>45961</v>
+      </c>
       <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="22"/>
+      <c r="D42" s="32">
+        <v>10</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>82</v>
+      </c>
       <c r="G42" s="39"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="63" t="str">
+      <c r="A43" s="63">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B43" s="34">
+        <v>45961</v>
+      </c>
       <c r="C43" s="35"/>
       <c r="D43" s="36"/>
       <c r="E43" s="37"/>
@@ -11407,11 +11442,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11419,11 +11454,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>2 h 00 min</v>
+        <v>2 h 20 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>9.125475285171103E-2</v>
+        <v>0.10071942446043165</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11444,11 +11479,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>380</v>
+        <v>425</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>845</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11456,11 +11491,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>13 h 20 min</v>
+        <v>14 h 05 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.60836501901140683</v>
+        <v>0.6079136690647482</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11497,7 +11532,7 @@
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>9.125475285171103E-2</v>
+        <v>8.6330935251798566E-2</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11518,11 +11553,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11530,11 +11565,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 35 min</v>
+        <v>4 h 45 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.20912547528517111</v>
+        <v>0.20503597122302158</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11590,22 +11625,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>775</v>
+        <v>850</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>1315</v>
+        <v>1390</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>21 h 55 min</v>
+        <v>23 h 10 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.91319444444444442</v>
+        <v>0.96527777777777779</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11649,6 +11684,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11657,15 +11701,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11870,6 +11905,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11878,14 +11921,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
src/ api(EnforceRateLimitAsync), supprimé api request de combobox
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A6223-1FE1-42C2-A0EA-457D23CBC8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1597B19B-8391-4D63-8F75-505221655BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>Auteur:</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>retouches du readme, Fix links and improve README formatting</t>
+  </si>
+  <si>
+    <t>src/ api(EnforceRateLimitAsync), supprimé api request de combobox</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1332,7 @@
                   <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>845</c:v>
+                  <c:v>875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>120</c:v>
@@ -2259,16 +2262,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.10071942446043165</c:v>
+                  <c:v>9.8591549295774641E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6079136690647482</c:v>
+                  <c:v>0.61619718309859151</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.6330935251798566E-2</c:v>
+                  <c:v>8.4507042253521125E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20503597122302158</c:v>
+                  <c:v>0.20070422535211269</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4456,8 +4459,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="6" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4512,7 +4515,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>23 heures 10 minutes</v>
+        <v>23 heures 40 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4531,11 +4534,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>850</v>
+        <v>880</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>1390</v>
+        <v>1420</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5419,9 +5422,15 @@
         <v>45961</v>
       </c>
       <c r="C43" s="35"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="22"/>
+      <c r="D43" s="36">
+        <v>30</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>83</v>
+      </c>
       <c r="G43" s="40"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -11458,7 +11467,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.10071942446043165</v>
+        <v>9.8591549295774641E-2</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11479,11 +11488,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>425</v>
+        <v>455</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>845</v>
+        <v>875</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11491,11 +11500,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>14 h 05 min</v>
+        <v>14 h 35 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.6079136690647482</v>
+        <v>0.61619718309859151</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11532,7 +11541,7 @@
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>8.6330935251798566E-2</v>
+        <v>8.4507042253521125E-2</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11569,7 +11578,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.20503597122302158</v>
+        <v>0.20070422535211269</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11625,22 +11634,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>850</v>
+        <v>880</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>1390</v>
+        <v>1420</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>23 h 10 min</v>
+        <v>23 h 40 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.96527777777777779</v>
+        <v>0.98611111111111116</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
chore(JDT) + schema de fonctionnement d'application
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Plot_those_lines\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1597B19B-8391-4D63-8F75-505221655BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872E52EC-84BD-42DB-BDD7-4D54FF836627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>Auteur:</t>
   </si>
@@ -1338,7 +1338,7 @@
                   <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>285</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2262,16 +2262,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.8591549295774641E-2</c:v>
+                  <c:v>9.6885813148788927E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61619718309859151</c:v>
+                  <c:v>0.60553633217993075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4507042253521125E-2</c:v>
+                  <c:v>8.3044982698961933E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20070422535211269</c:v>
+                  <c:v>0.21453287197231835</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4458,9 +4458,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4515,7 +4515,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>23 heures 40 minutes</v>
+        <v>24 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4534,11 +4534,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>880</v>
+        <v>905</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>1420</v>
+        <v>1445</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5434,27 +5434,43 @@
       <c r="G43" s="40"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="62" t="str">
+      <c r="A44" s="62">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B44" s="30">
+        <v>45961</v>
+      </c>
       <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="22"/>
+      <c r="D44" s="32">
+        <v>10</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="G44" s="39"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="63" t="str">
+      <c r="A45" s="63">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="34">
+        <v>45961</v>
+      </c>
       <c r="C45" s="35"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="22"/>
+      <c r="D45" s="36">
+        <v>15</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>73</v>
+      </c>
       <c r="G45" s="40"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -11467,7 +11483,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>9.8591549295774641E-2</v>
+        <v>9.6885813148788927E-2</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11504,7 +11520,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.61619718309859151</v>
+        <v>0.60553633217993075</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11541,7 +11557,7 @@
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>8.4507042253521125E-2</v>
+        <v>8.3044982698961933E-2</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11562,11 +11578,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11574,11 +11590,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 45 min</v>
+        <v>5 h 10 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.20070422535211269</v>
+        <v>0.21453287197231835</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11634,22 +11650,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>880</v>
+        <v>905</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>1420</v>
+        <v>1445</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>23 h 40 min</v>
+        <v>24 h 05 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.98611111111111116</v>
+        <v>1.0034722222222223</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11693,15 +11709,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11710,6 +11717,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11914,14 +11930,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11930,6 +11938,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>